<commit_message>
50 steps traj MLP
</commit_message>
<xml_diff>
--- a/experiments/pg/return_discount_increment/baseline_max_rew_mlp_3x182_small_batch_30k_epochs_eps_1e_8_alpha_ret_0/oracle_buffer.xlsx
+++ b/experiments/pg/return_discount_increment/baseline_max_rew_mlp_3x182_small_batch_30k_epochs_eps_1e_8_alpha_ret_0/oracle_buffer.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C368"/>
+  <dimension ref="A1:C369"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5216,6 +5216,19 @@
         <v>16.21057970074723</v>
       </c>
     </row>
+    <row r="369">
+      <c r="A369" s="1" t="n">
+        <v>367</v>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>[3, -1, 1]</t>
+        </is>
+      </c>
+      <c r="C369" t="n">
+        <v>16.80110331690178</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>